<commit_message>
still working on insert operation
</commit_message>
<xml_diff>
--- a/ITSM_Dashboard_Business_Requirements/Diagrams.xlsx
+++ b/ITSM_Dashboard_Business_Requirements/Diagrams.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Node\ITSMDashboard\ITSMDashboard_React\ITSM_Dashboard_Business_Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD29F797-0DF3-473E-B554-0ADD3B20C8C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5F64F1-8D1A-43B4-A98D-4406D8C97EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B05F46BE-C4B9-4C9E-807D-50EBDEC42364}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{B05F46BE-C4B9-4C9E-807D-50EBDEC42364}"/>
   </bookViews>
   <sheets>
     <sheet name="Download" sheetId="1" r:id="rId1"/>
     <sheet name="Delete" sheetId="3" r:id="rId2"/>
+    <sheet name="Tech_Data_Flow" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -3397,6 +3398,1350 @@
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="Rectangle 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A22872B-8261-C63E-1B9A-A777E92B5148}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="586740" y="807720"/>
+          <a:ext cx="1112520" cy="1310640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Database </a:t>
+          </a:r>
+          <a:endParaRPr lang="LID4096" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>295966</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>34345</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>189285</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>64824</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="Rectangle 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C0DEDD4-BFB5-40F4-96E5-FAF565A30D8B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2725531" y="973041"/>
+          <a:ext cx="1108102" cy="1344653"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>ORM</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>  Model,Seqalize</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>(Transaction rollback, DB lock)</a:t>
+          </a:r>
+          <a:endParaRPr lang="LID4096" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>471335</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>41192</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>364656</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>71671</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="Rectangle 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D92B3032-2A6E-4F1A-B546-88750FAB37B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4115683" y="979888"/>
+          <a:ext cx="1108103" cy="1344653"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>API</a:t>
+          </a:r>
+          <a:endParaRPr lang="LID4096" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>994</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>3864</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>66261</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>3865</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="Rectangle 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A99C141-3197-4F75-A0F1-782CFDDA61FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2430559" y="754821"/>
+          <a:ext cx="4317006" cy="1877392"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="22225"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="LID4096" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>100054</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>123024</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>273105</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>176364</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="TextBox 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBF06EE3-AEA0-4EB2-B4AB-5D5E5251A6D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3744402" y="498502"/>
+          <a:ext cx="780442" cy="241079"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Express</a:t>
+          </a:r>
+          <a:endParaRPr lang="LID4096" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>185310</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>295966</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>143455</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Connector: Elbow 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E1428A3-B176-BD9F-8A53-18BC6B53DF61}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="29" idx="3"/>
+          <a:endCxn id="31" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1694843" y="1499484"/>
+          <a:ext cx="1030688" cy="145884"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>242624</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>150302</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>471334</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>64824</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Connector: Elbow 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31CAA10B-C649-4FDF-B23A-70E7CC2A4381}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="31" idx="2"/>
+          <a:endCxn id="32" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="3364892" y="1566904"/>
+          <a:ext cx="665479" cy="836101"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -34351"/>
+            <a:gd name="adj2" fmla="val 83133"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>88348</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="Rectangle 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97B1F97B-46B1-4190-96BC-6E52C07BF1BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7387756" y="723237"/>
+          <a:ext cx="5455809" cy="1877392"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="22225"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="LID4096" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="TextBox 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40CDB540-3578-4B39-A084-32CCE5D1B605}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8808720" y="457200"/>
+          <a:ext cx="784860" cy="236220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>React</a:t>
+          </a:r>
+          <a:endParaRPr lang="LID4096" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="Rectangle 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05AC81FE-FF3E-4F4C-9A18-98641DFBBB48}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7658100" y="944880"/>
+          <a:ext cx="1112520" cy="1310640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>RTX query</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Slice</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>(Caching, Incrimenta ritreval)</a:t>
+          </a:r>
+          <a:endParaRPr lang="LID4096" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="Rectangle 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE41792F-E0FA-4081-AF78-6084685920C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8976360" y="937260"/>
+          <a:ext cx="1112520" cy="1310640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>React Component</a:t>
+          </a:r>
+          <a:endParaRPr lang="LID4096" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>531854</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>29707</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>425174</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>60187</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="Rectangle 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{477F4520-7EA8-4E41-BD3C-9CD654CE0EA8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10250115" y="968403"/>
+          <a:ext cx="1108102" cy="1344654"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>React Router/File router</a:t>
+          </a:r>
+          <a:endParaRPr lang="LID4096" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>59193</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>5411</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>559904</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>35891</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="Rectangle 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4D0261E-F795-4196-9893-CFA2F4A54636}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11599628" y="944107"/>
+          <a:ext cx="1108102" cy="1344654"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>React entrypoint Index.js</a:t>
+          </a:r>
+          <a:endParaRPr lang="LID4096" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>66555</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>107379</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>569474</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>137859</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="Rectangle 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A092469-C90C-45F4-BF32-D2B5895804BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13477755" y="1038712"/>
+          <a:ext cx="1112519" cy="1334347"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Browser/Addin</a:t>
+          </a:r>
+          <a:endParaRPr lang="LID4096" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>27388</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>61070</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>528100</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>91549</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="51" name="Rectangle 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED79F75D-9CAE-41D2-95B9-408818381B81}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5493910" y="999766"/>
+          <a:ext cx="1108103" cy="1344653"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>EXpress router /Network Router</a:t>
+          </a:r>
+          <a:endParaRPr lang="LID4096" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>417995</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>170180</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>27387</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>71671</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="53" name="Connector: Elbow 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B33E592F-85CD-42C0-8C62-86E29BE71E76}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="32" idx="2"/>
+          <a:endCxn id="51" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="4755598" y="1586229"/>
+          <a:ext cx="652448" cy="824175"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -35037"/>
+            <a:gd name="adj2" fmla="val 83612"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>528100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>139590</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>170180</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="57" name="Connector: Elbow 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F0B73BB-AF73-4AAC-A205-05BCAF0D9FC3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="51" idx="3"/>
+          <a:endCxn id="42" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6602013" y="1641503"/>
+          <a:ext cx="1029583" cy="30590"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>289559</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>131970</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>441959</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="60" name="Connector: Elbow 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6B3C096-D242-4E4E-AE88-D19653DE5F0B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="42" idx="2"/>
+          <a:endCxn id="43" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="8225568" y="1593961"/>
+          <a:ext cx="679947" cy="759791"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -33620"/>
+            <a:gd name="adj2" fmla="val 86461"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>388619</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>138817</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>531853</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="63" name="Connector: Elbow 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0012DEAC-05D4-437A-8345-E05FDAC253CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="43" idx="2"/>
+          <a:endCxn id="46" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="9542062" y="1598157"/>
+          <a:ext cx="665480" cy="750625"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -34351"/>
+            <a:gd name="adj2" fmla="val 86906"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>478514</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>114521</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>59193</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>60187</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="66" name="Connector: Elbow 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47783ED2-E74E-4E7C-825C-B1AD4784F3AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="46" idx="2"/>
+          <a:endCxn id="47" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="10853585" y="1567015"/>
+          <a:ext cx="696623" cy="795462"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -32815"/>
+            <a:gd name="adj2" fmla="val 84826"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>559904</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>113785</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>66555</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>29486</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="69" name="Connector: Elbow 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0760F02C-2DCE-4ACD-A33B-EB1DA15D2682}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="47" idx="3"/>
+          <a:endCxn id="48" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12751904" y="1603918"/>
+          <a:ext cx="725851" cy="101968"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
           <a:tailEnd type="triangle"/>
         </a:ln>
       </xdr:spPr>
@@ -3739,7 +5084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D53C781-2C0B-4C2C-B413-933FDA7DE92D}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
@@ -3773,4 +5118,24 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2A4AFA-194A-46C1-96BB-FDA3B2FAAE2A}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="S23" sqref="S23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="4" customFormat="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
did mutiple rtk query working
</commit_message>
<xml_diff>
--- a/ITSM_Dashboard_Business_Requirements/Diagrams.xlsx
+++ b/ITSM_Dashboard_Business_Requirements/Diagrams.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Node\ITSMDashboard\ITSMDashboard_React\ITSM_Dashboard_Business_Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DA612C-7D5E-4BF2-A709-FD7619BC7EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A17028-9FE1-49C1-B91A-90F59C81C9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="38670" windowHeight="21150" activeTab="2" xr2:uid="{B05F46BE-C4B9-4C9E-807D-50EBDEC42364}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{B05F46BE-C4B9-4C9E-807D-50EBDEC42364}"/>
   </bookViews>
   <sheets>
     <sheet name="Download" sheetId="1" r:id="rId1"/>
-    <sheet name="Delete" sheetId="3" r:id="rId2"/>
-    <sheet name="Tech_Data_Flow" sheetId="5" r:id="rId3"/>
+    <sheet name="debt" sheetId="6" r:id="rId2"/>
+    <sheet name="Delete" sheetId="3" r:id="rId3"/>
+    <sheet name="Tech_Data_Flow" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,6 +36,26 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>delete with filter</t>
+  </si>
+  <si>
+    <t>encrytion of payload</t>
+  </si>
+  <si>
+    <t>refactor all api to HTTPS</t>
+  </si>
+  <si>
+    <t>Fill patern in a cell</t>
+  </si>
+  <si>
+    <t>https://sproutsocial.com/insights/linkedin-business-page/</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5165,6 +5186,49 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93A746C3-7EB2-405D-A219-C7B5E8792639}">
+  <dimension ref="C2:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="71.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC96BA80-82E3-4D6F-97CF-7D5BBC9274C2}">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -5184,11 +5248,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2A4AFA-194A-46C1-96BB-FDA3B2FAAE2A}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <selection activeCell="Z15" sqref="Z15"/>
     </sheetView>
   </sheetViews>

</xml_diff>